<commit_message>
document import files updated (#1t1uf4t)
</commit_message>
<xml_diff>
--- a/public/files/import/bills.xlsx
+++ b/public/files/import/bills.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="7070" tabRatio="500" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12575" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="bills" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
   <si>
     <t>bill_number</t>
   </si>
@@ -64,6 +64,18 @@
     <t>contact_address</t>
   </si>
   <si>
+    <t>contact_country</t>
+  </si>
+  <si>
+    <t>contact_state</t>
+  </si>
+  <si>
+    <t>contact_zip_code</t>
+  </si>
+  <si>
+    <t>contact_city</t>
+  </si>
+  <si>
     <t>notes</t>
   </si>
   <si>
@@ -88,7 +100,10 @@
     <t>test@vendor.com</t>
   </si>
   <si>
-    <t>Ut.</t>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Est.</t>
   </si>
   <si>
     <t>item_name</t>
@@ -171,11 +186,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -183,6 +198,44 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -190,77 +243,71 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -272,70 +319,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -350,85 +365,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,97 +521,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -541,6 +556,45 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -555,15 +609,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -583,41 +628,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -644,144 +659,144 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1101,31 +1116,33 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
-    <col min="2" max="2" width="15.2818181818182" customWidth="1"/>
-    <col min="3" max="3" width="8.13636363636364" customWidth="1"/>
-    <col min="4" max="5" width="12.8545454545455" customWidth="1"/>
-    <col min="6" max="6" width="8.13636363636364" customWidth="1"/>
-    <col min="7" max="8" width="16.4272727272727" customWidth="1"/>
+    <col min="2" max="2" width="15.2777777777778" customWidth="1"/>
+    <col min="3" max="3" width="8.13888888888889" customWidth="1"/>
+    <col min="4" max="5" width="12.8518518518519" customWidth="1"/>
+    <col min="6" max="6" width="8.13888888888889" customWidth="1"/>
+    <col min="7" max="8" width="16.4259259259259" customWidth="1"/>
     <col min="9" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="15.2818181818182" customWidth="1"/>
-    <col min="11" max="11" width="18.7090909090909" customWidth="1"/>
-    <col min="12" max="12" width="22.2818181818182" customWidth="1"/>
-    <col min="13" max="13" width="16.4272727272727" customWidth="1"/>
-    <col min="14" max="14" width="18.7090909090909" customWidth="1"/>
-    <col min="15" max="15" width="7" customWidth="1"/>
-    <col min="16" max="16" width="8.13636363636364" customWidth="1"/>
+    <col min="10" max="10" width="15.2777777777778" customWidth="1"/>
+    <col min="11" max="11" width="18.712962962963" customWidth="1"/>
+    <col min="12" max="12" width="22.2777777777778" customWidth="1"/>
+    <col min="13" max="13" width="16.4259259259259" customWidth="1"/>
+    <col min="14" max="14" width="18.712962962963" customWidth="1"/>
+    <col min="15" max="15" width="15.7777777777778" customWidth="1"/>
+    <col min="16" max="16" width="13.4444444444444" customWidth="1"/>
+    <col min="17" max="17" width="16.8888888888889" customWidth="1"/>
+    <col min="18" max="18" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1174,13 +1191,25 @@
       <c r="P1" t="s">
         <v>15</v>
       </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:15">
+    <row r="2" spans="1:19">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1">
         <v>43831</v>
@@ -1192,22 +1221,25 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H2">
         <v>1</v>
       </c>
       <c r="I2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="K2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="O2" t="s">
-        <v>22</v>
+        <v>26</v>
+      </c>
+      <c r="S2" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -1226,13 +1258,13 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
   <cols>
-    <col min="1" max="1" width="11.9090909090909" customWidth="1"/>
-    <col min="2" max="2" width="11.7090909090909" customWidth="1"/>
-    <col min="3" max="3" width="10.5727272727273" customWidth="1"/>
+    <col min="1" max="1" width="11.9074074074074" customWidth="1"/>
+    <col min="2" max="2" width="11.712962962963" customWidth="1"/>
+    <col min="3" max="3" width="10.5740740740741" customWidth="1"/>
     <col min="4" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="4.57272727272727" customWidth="1"/>
+    <col min="6" max="6" width="4.57407407407407" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1240,27 +1272,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="E1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -1284,16 +1316,16 @@
   <sheetPr/>
   <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="11.9090909090909" customWidth="1"/>
-    <col min="2" max="2" width="15.2818181818182" customWidth="1"/>
-    <col min="3" max="3" width="8.13636363636364" customWidth="1"/>
-    <col min="4" max="4" width="5.84545454545455" customWidth="1"/>
+    <col min="1" max="1" width="11.9074074074074" customWidth="1"/>
+    <col min="2" max="2" width="15.2777777777778" customWidth="1"/>
+    <col min="3" max="3" width="8.13888888888889" customWidth="1"/>
+    <col min="4" max="4" width="5.84259259259259" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1301,10 +1333,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -1326,11 +1358,11 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="11.9090909090909" customWidth="1"/>
-    <col min="2" max="3" width="8.13636363636364" customWidth="1"/>
-    <col min="4" max="4" width="17.5636363636364" customWidth="1"/>
+    <col min="1" max="1" width="11.9074074074074" customWidth="1"/>
+    <col min="2" max="3" width="8.13888888888889" customWidth="1"/>
+    <col min="4" max="4" width="17.5648148148148" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1341,32 +1373,32 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1385,13 +1417,13 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="11.9090909090909" customWidth="1"/>
-    <col min="2" max="2" width="11.7090909090909" customWidth="1"/>
-    <col min="3" max="3" width="18.7090909090909" customWidth="1"/>
-    <col min="4" max="4" width="8.13636363636364" customWidth="1"/>
-    <col min="5" max="5" width="12.8545454545455" customWidth="1"/>
+    <col min="1" max="1" width="11.9074074074074" customWidth="1"/>
+    <col min="2" max="2" width="11.712962962963" customWidth="1"/>
+    <col min="3" max="3" width="18.712962962963" customWidth="1"/>
+    <col min="4" max="4" width="8.13888888888889" customWidth="1"/>
+    <col min="5" max="5" width="12.8518518518519" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1399,27 +1431,27 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -1430,13 +1462,13 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -1461,18 +1493,18 @@
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="11.9090909090909" customWidth="1"/>
-    <col min="2" max="2" width="12.8545454545455" customWidth="1"/>
-    <col min="3" max="3" width="8.13636363636364" customWidth="1"/>
-    <col min="4" max="5" width="16.4272727272727" customWidth="1"/>
-    <col min="6" max="6" width="14.3636363636364" customWidth="1"/>
-    <col min="7" max="7" width="17.2818181818182" customWidth="1"/>
+    <col min="1" max="1" width="11.9074074074074" customWidth="1"/>
+    <col min="2" max="2" width="12.8518518518519" customWidth="1"/>
+    <col min="3" max="3" width="8.13888888888889" customWidth="1"/>
+    <col min="4" max="5" width="16.4259259259259" customWidth="1"/>
+    <col min="6" max="6" width="14.3611111111111" customWidth="1"/>
+    <col min="7" max="7" width="17.2777777777778" customWidth="1"/>
     <col min="8" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="28.1363636363636" customWidth="1"/>
-    <col min="11" max="11" width="11.7090909090909" customWidth="1"/>
-    <col min="12" max="12" width="12.8545454545455" customWidth="1"/>
+    <col min="10" max="10" width="28.1388888888889" customWidth="1"/>
+    <col min="11" max="11" width="11.712962962963" customWidth="1"/>
+    <col min="12" max="12" width="12.8518518518519" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1480,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -1492,7 +1524,7 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G1" t="s">
         <v>10</v>
@@ -1501,21 +1533,21 @@
         <v>8</v>
       </c>
       <c r="I1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="J1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="K1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="L1" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1">
         <v>43831</v>
@@ -1524,22 +1556,22 @@
         <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="J2" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
import sample files updated
</commit_message>
<xml_diff>
--- a/public/files/import/bills.xlsx
+++ b/public/files/import/bills.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="500"/>
+    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="bills" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
   <si>
     <t>bill_number</t>
   </si>
@@ -160,6 +160,9 @@
     <t>bills.total</t>
   </si>
   <si>
+    <t>transaction_number</t>
+  </si>
+  <si>
     <t>paid_at</t>
   </si>
   <si>
@@ -173,6 +176,9 @@
   </si>
   <si>
     <t>reconciled</t>
+  </si>
+  <si>
+    <t>TRA-00001</t>
   </si>
   <si>
     <t>Cash</t>
@@ -186,18 +192,47 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -206,19 +241,36 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -228,47 +280,25 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -280,6 +310,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -288,69 +340,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -365,187 +377,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -560,55 +572,16 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
         <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -632,16 +605,55 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -659,144 +671,145 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="180" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1118,7 +1131,7 @@
   <sheetPr/>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -1487,56 +1500,56 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="11.9074074074074" customWidth="1"/>
-    <col min="2" max="2" width="12.8518518518519" customWidth="1"/>
-    <col min="3" max="3" width="8.13888888888889" customWidth="1"/>
-    <col min="4" max="5" width="16.4259259259259" customWidth="1"/>
-    <col min="6" max="6" width="14.3611111111111" customWidth="1"/>
-    <col min="7" max="7" width="17.2777777777778" customWidth="1"/>
-    <col min="8" max="9" width="14" customWidth="1"/>
-    <col min="10" max="10" width="28.1388888888889" customWidth="1"/>
-    <col min="11" max="11" width="11.712962962963" customWidth="1"/>
-    <col min="12" max="12" width="12.8518518518519" customWidth="1"/>
+    <col min="1" max="2" width="11.9074074074074" customWidth="1"/>
+    <col min="3" max="3" width="12.8518518518519" customWidth="1"/>
+    <col min="4" max="4" width="8.13888888888889" customWidth="1"/>
+    <col min="5" max="6" width="16.4259259259259" customWidth="1"/>
+    <col min="7" max="7" width="14.3611111111111" customWidth="1"/>
+    <col min="8" max="8" width="17.2777777777778" customWidth="1"/>
+    <col min="9" max="10" width="14" customWidth="1"/>
+    <col min="11" max="11" width="28.1388888888889" customWidth="1"/>
+    <col min="12" max="12" width="11.712962962963" customWidth="1"/>
+    <col min="13" max="13" width="12.8518518518519" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:13">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
-        <v>47</v>
-      </c>
       <c r="G1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>36</v>
-      </c>
-      <c r="J1" t="s">
-        <v>48</v>
       </c>
       <c r="K1" t="s">
         <v>49</v>
@@ -1544,34 +1557,40 @@
       <c r="L1" t="s">
         <v>50</v>
       </c>
+      <c r="M1" t="s">
+        <v>51</v>
+      </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="1">
         <v>43831</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>22</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>51</v>
-      </c>
       <c r="G2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>23</v>
       </c>
-      <c r="J2" t="s">
-        <v>52</v>
+      <c r="K2" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issue of importing invoice and bill refs #2710
</commit_message>
<xml_diff>
--- a/public/files/import/bills.xlsx
+++ b/public/files/import/bills.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="500" activeTab="5"/>
+    <workbookView windowWidth="23040" windowHeight="9215" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bills" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
   <si>
     <t>bill_number</t>
   </si>
@@ -109,6 +109,9 @@
     <t>item_name</t>
   </si>
   <si>
+    <t>item_type</t>
+  </si>
+  <si>
     <t>quantity</t>
   </si>
   <si>
@@ -121,7 +124,13 @@
     <t>tax</t>
   </si>
   <si>
+    <t>BILL-00001</t>
+  </si>
+  <si>
     <t>Test Item</t>
+  </si>
+  <si>
+    <t>product</t>
   </si>
   <si>
     <t>tax_rate</t>
@@ -212,8 +221,88 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -227,68 +316,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -302,67 +332,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -377,37 +386,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -419,145 +560,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,21 +577,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -604,30 +598,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -639,6 +609,15 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -658,6 +637,36 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -671,138 +680,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1265,22 +1274,24 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="11.9074074074074" customWidth="1"/>
     <col min="2" max="2" width="11.712962962963" customWidth="1"/>
     <col min="3" max="3" width="10.5740740740741" customWidth="1"/>
-    <col min="4" max="5" width="7" customWidth="1"/>
-    <col min="6" max="6" width="4.57407407407407" customWidth="1"/>
+    <col min="4" max="4" width="7.66666666666667" customWidth="1"/>
+    <col min="5" max="5" width="5.11111111111111" customWidth="1"/>
+    <col min="6" max="6" width="5.77777777777778" customWidth="1"/>
+    <col min="7" max="7" width="5.44444444444444" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1299,21 +1310,27 @@
       <c r="F1" t="s">
         <v>32</v>
       </c>
+      <c r="G1" t="s">
+        <v>33</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2">
         <v>1</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>10</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>10</v>
       </c>
     </row>
@@ -1349,7 +1366,7 @@
         <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -1386,10 +1403,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1397,10 +1414,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1411,7 +1428,7 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1444,16 +1461,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1461,10 +1478,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -1478,10 +1495,10 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -1502,7 +1519,7 @@
   <sheetPr/>
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1525,10 +1542,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -1540,7 +1557,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="H1" t="s">
         <v>10</v>
@@ -1549,16 +1566,16 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="K1" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="L1" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="M1" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1566,7 +1583,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C2" s="1">
         <v>43831</v>
@@ -1581,7 +1598,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
@@ -1590,7 +1607,7 @@
         <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update example excel files
</commit_message>
<xml_diff>
--- a/public/files/import/bills.xlsx
+++ b/public/files/import/bills.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9215" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="22368" windowHeight="9215" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="bills" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
   <si>
     <t>bill_number</t>
   </si>
@@ -109,6 +109,9 @@
     <t>item_name</t>
   </si>
   <si>
+    <t>item_description</t>
+  </si>
+  <si>
     <t>item_type</t>
   </si>
   <si>
@@ -128,6 +131,9 @@
   </si>
   <si>
     <t>Test Item</t>
+  </si>
+  <si>
+    <t>test bill item</t>
   </si>
   <si>
     <t>product</t>
@@ -201,10 +207,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="23">
@@ -221,50 +227,43 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -324,6 +323,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -333,45 +339,45 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -386,13 +392,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -404,169 +554,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -585,15 +591,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -652,6 +649,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -680,138 +686,138 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="178" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1274,24 +1280,24 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
     <col min="1" max="1" width="11.9074074074074" customWidth="1"/>
     <col min="2" max="2" width="11.712962962963" customWidth="1"/>
-    <col min="3" max="3" width="10.5740740740741" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="7.66666666666667" customWidth="1"/>
     <col min="5" max="5" width="5.11111111111111" customWidth="1"/>
     <col min="6" max="6" width="5.77777777777778" customWidth="1"/>
     <col min="7" max="7" width="5.44444444444444" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1313,24 +1319,30 @@
       <c r="G1" t="s">
         <v>33</v>
       </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D2">
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2">
         <v>1</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>10</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>10</v>
       </c>
     </row>
@@ -1366,7 +1378,7 @@
         <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -1403,10 +1415,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1414,10 +1426,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1428,7 +1440,7 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1461,16 +1473,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1478,10 +1490,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -1495,10 +1507,10 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -1542,10 +1554,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -1557,7 +1569,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s">
         <v>10</v>
@@ -1566,16 +1578,16 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="K1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="L1" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="M1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1583,7 +1595,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1">
         <v>43831</v>
@@ -1598,7 +1610,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
@@ -1607,7 +1619,7 @@
         <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated bill sample export file
</commit_message>
<xml_diff>
--- a/public/files/import/bills.xlsx
+++ b/public/files/import/bills.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="22368" windowHeight="9215" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="22368" windowHeight="9215" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="bills" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>bill_number</t>
   </si>
@@ -82,7 +82,7 @@
     <t>footer</t>
   </si>
   <si>
-    <t>BIL-12345</t>
+    <t>BILL-00001</t>
   </si>
   <si>
     <t>paid</t>
@@ -125,9 +125,6 @@
   </si>
   <si>
     <t>tax</t>
-  </si>
-  <si>
-    <t>BILL-00001</t>
   </si>
   <si>
     <t>Test Item</t>
@@ -207,11 +204,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="178" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="180" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -228,7 +225,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -236,15 +233,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -256,30 +245,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -294,14 +267,61 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -315,16 +335,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -338,46 +372,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -392,19 +389,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,25 +545,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -446,133 +569,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -583,78 +580,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -675,6 +600,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -683,99 +617,192 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="179" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -784,46 +811,16 @@
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1146,8 +1143,8 @@
   <sheetPr/>
   <dimension ref="A1:T2"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1282,8 +1279,8 @@
   <sheetPr/>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1" outlineLevelCol="7"/>
@@ -1325,16 +1322,16 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" t="s">
         <v>36</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>38</v>
       </c>
       <c r="E2">
         <v>1</v>
@@ -1359,7 +1356,7 @@
   <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="3"/>
@@ -1378,7 +1375,7 @@
         <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -1397,7 +1394,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="3"/>
@@ -1415,10 +1412,10 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
         <v>40</v>
-      </c>
-      <c r="D1" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1426,10 +1423,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D2" t="s">
         <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1440,7 +1437,7 @@
         <v>21</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -1456,7 +1453,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="4"/>
@@ -1473,16 +1470,16 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
         <v>45</v>
-      </c>
-      <c r="C1" t="s">
-        <v>46</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1490,10 +1487,10 @@
         <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" t="s">
         <v>48</v>
-      </c>
-      <c r="C2" t="s">
-        <v>49</v>
       </c>
       <c r="D2">
         <v>10</v>
@@ -1510,7 +1507,7 @@
         <v>33</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3">
         <v>10</v>
@@ -1532,7 +1529,7 @@
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelRow="1"/>
@@ -1554,10 +1551,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" t="s">
         <v>51</v>
-      </c>
-      <c r="C1" t="s">
-        <v>52</v>
       </c>
       <c r="D1" t="s">
         <v>5</v>
@@ -1569,7 +1566,7 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H1" t="s">
         <v>10</v>
@@ -1578,16 +1575,16 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K1" t="s">
+        <v>53</v>
+      </c>
+      <c r="L1" t="s">
         <v>54</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>55</v>
-      </c>
-      <c r="M1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1595,7 +1592,7 @@
         <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C2" s="1">
         <v>43831</v>
@@ -1610,7 +1607,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
@@ -1619,7 +1616,7 @@
         <v>23</v>
       </c>
       <c r="K2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>